<commit_message>
Change notes generation method
</commit_message>
<xml_diff>
--- a/data/tables/main.xlsx
+++ b/data/tables/main.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgcha\Desktop\Python\Códigos\tsakonian_dictionary_app\data\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE4103E9-5F00-4389-A4AA-74DDDF36636B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340F3432-D28D-4F58-9FBE-7EA695411581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13260" yWindow="0" windowWidth="15645" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3107" uniqueCount="1957">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3108" uniqueCount="1957">
   <si>
     <t>tsakonian</t>
   </si>
@@ -6255,8 +6255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D1073"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1047" zoomScale="131" workbookViewId="0">
-      <selection activeCell="A1073" sqref="A1073"/>
+    <sheetView tabSelected="1" topLeftCell="A583" zoomScale="131" workbookViewId="0">
+      <selection activeCell="C616" sqref="C616"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14621,6 +14621,9 @@
       <c r="B615" t="s">
         <v>1168</v>
       </c>
+      <c r="C615" t="s">
+        <v>44</v>
+      </c>
       <c r="D615">
         <v>1</v>
       </c>

</xml_diff>